<commit_message>
import/export testing for question data
</commit_message>
<xml_diff>
--- a/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
+++ b/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="160" windowWidth="24880" windowHeight="15980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15760"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="3" r:id="rId1"/>
@@ -346,7 +346,7 @@
     <t>answer_exercise_longjump</t>
   </si>
   <si>
-    <t>11</t>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -455,10 +455,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -825,9 +825,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -837,7 +837,7 @@
     <col min="3" max="3" width="29.83203125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="4.5" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="39.5" customWidth="1"/>
@@ -881,19 +881,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
@@ -1119,23 +1119,23 @@
       </c>
     </row>
     <row r="22" spans="1:16" s="2" customFormat="1">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="6" t="s">
-        <v>25</v>
+      <c r="A24" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="B24" t="s">
         <v>78</v>
@@ -1205,8 +1205,8 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="6" t="s">
-        <v>26</v>
+      <c r="A29" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="B29" t="s">
         <v>105</v>
@@ -1228,8 +1228,8 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="6" t="s">
-        <v>27</v>
+      <c r="A31" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B31" t="s">
         <v>106</v>
@@ -1271,23 +1271,23 @@
       </c>
     </row>
     <row r="34" spans="1:16" s="2" customFormat="1">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="6" t="s">
-        <v>14</v>
+      <c r="A36" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B36" t="s">
         <v>86</v>
@@ -1334,8 +1334,8 @@
       </c>
     </row>
     <row r="40" spans="1:16">
-      <c r="A40" s="6" t="s">
-        <v>108</v>
+      <c r="A40" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="B40" t="s">
         <v>94</v>
@@ -1410,7 +1410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>

</xml_diff>

<commit_message>
read answers excel file from original
</commit_message>
<xml_diff>
--- a/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
+++ b/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="109">
   <si>
     <t>id</t>
   </si>
@@ -416,8 +416,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -460,7 +462,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -475,6 +477,7 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -489,6 +492,7 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -826,8 +830,8 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1346,8 +1350,8 @@
       <c r="D40" t="s">
         <v>10</v>
       </c>
-      <c r="F40">
-        <v>2</v>
+      <c r="F40" t="s">
+        <v>11</v>
       </c>
       <c r="H40" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
have export test use the questions xlsx file instead of csv file
</commit_message>
<xml_diff>
--- a/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
+++ b/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>5</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>2</t>
@@ -416,7 +413,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -448,8 +445,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -461,8 +476,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -478,6 +494,15 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -493,6 +518,15 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -829,9 +863,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -851,37 +885,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>39</v>
-      </c>
-      <c r="K1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1">
@@ -904,7 +938,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -915,11 +949,8 @@
       <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J5">
         <v>10</v>
@@ -930,25 +961,25 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
         <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
-        <v>53</v>
       </c>
       <c r="J7">
         <v>10</v>
@@ -957,10 +988,10 @@
     <row r="8" spans="1:11">
       <c r="A8" s="4"/>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J8">
         <v>20</v>
@@ -969,10 +1000,10 @@
     <row r="9" spans="1:11">
       <c r="A9" s="4"/>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J9">
         <v>30</v>
@@ -983,25 +1014,25 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="I11" t="s">
         <v>57</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" t="s">
-        <v>58</v>
       </c>
       <c r="J11">
         <v>10</v>
@@ -1010,10 +1041,10 @@
     <row r="12" spans="1:11">
       <c r="A12" s="4"/>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J12">
         <v>20</v>
@@ -1024,25 +1055,22 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="I14" t="s">
         <v>61</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" t="s">
-        <v>62</v>
       </c>
       <c r="J14">
         <v>10</v>
@@ -1051,10 +1079,10 @@
     <row r="15" spans="1:11">
       <c r="A15" s="4"/>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J15">
         <v>20</v>
@@ -1063,68 +1091,68 @@
     <row r="16" spans="1:11">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:12">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" t="s">
         <v>66</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" t="s">
-        <v>67</v>
       </c>
       <c r="J17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:12">
       <c r="H18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J18">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:12">
       <c r="H19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J19">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:12">
       <c r="H20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J20">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="2" customFormat="1">
+    <row r="22" spans="1:12" s="2" customFormat="1">
       <c r="A22" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1137,146 +1165,138 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:12">
       <c r="A24" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" t="s">
         <v>78</v>
       </c>
-      <c r="C24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" t="s">
-        <v>76</v>
-      </c>
-      <c r="F24" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" t="s">
-        <v>79</v>
-      </c>
       <c r="I24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J24">
         <v>10</v>
       </c>
       <c r="K24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="H25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J25">
         <v>20</v>
       </c>
       <c r="K25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="H26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J26">
         <v>30</v>
       </c>
       <c r="K26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="H27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J27">
         <v>40</v>
       </c>
       <c r="K27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" t="s">
         <v>25</v>
       </c>
-      <c r="B29" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="H29" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" t="s">
         <v>102</v>
-      </c>
-      <c r="F29" t="s">
-        <v>26</v>
-      </c>
-      <c r="H29" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" t="s">
-        <v>103</v>
       </c>
       <c r="J29">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:12">
       <c r="A31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" t="s">
         <v>26</v>
       </c>
-      <c r="B31" t="s">
+      <c r="H31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" t="s">
         <v>106</v>
-      </c>
-      <c r="C31" t="s">
-        <v>104</v>
-      </c>
-      <c r="F31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I31" t="s">
-        <v>107</v>
       </c>
       <c r="J31">
         <v>10</v>
       </c>
-      <c r="N31" t="s">
-        <v>10</v>
-      </c>
-      <c r="O31" t="s">
-        <v>10</v>
-      </c>
-      <c r="P31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
+    </row>
+    <row r="32" spans="1:12">
       <c r="H32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J32">
         <v>20</v>
       </c>
+      <c r="L32" s="7"/>
     </row>
     <row r="34" spans="1:16" s="2" customFormat="1">
       <c r="A34" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1291,25 +1311,22 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" t="s">
         <v>86</v>
       </c>
-      <c r="C36" t="s">
+      <c r="F36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" t="s">
         <v>87</v>
       </c>
-      <c r="D36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36" t="s">
-        <v>88</v>
-      </c>
       <c r="I36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J36">
         <v>10</v>
@@ -1317,10 +1334,10 @@
     </row>
     <row r="37" spans="1:16">
       <c r="H37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J37" s="1">
         <v>20</v>
@@ -1328,10 +1345,10 @@
     </row>
     <row r="38" spans="1:16">
       <c r="H38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J38" s="1">
         <v>30</v>
@@ -1339,60 +1356,55 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" t="s">
         <v>94</v>
       </c>
-      <c r="C40" t="s">
+      <c r="F40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" t="s">
         <v>95</v>
       </c>
-      <c r="D40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" t="s">
-        <v>96</v>
-      </c>
       <c r="I40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J40">
         <v>10</v>
       </c>
-      <c r="N40" t="s">
-        <v>10</v>
-      </c>
-      <c r="O40" t="s">
-        <v>10</v>
-      </c>
-      <c r="P40" t="s">
-        <v>10</v>
-      </c>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
     </row>
     <row r="41" spans="1:16">
       <c r="H41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J41">
         <v>20</v>
       </c>
+      <c r="L41" s="7"/>
     </row>
     <row r="42" spans="1:16">
       <c r="H42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J42">
         <v>30</v>
       </c>
+      <c r="L42" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1441,7 +1453,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1455,30 +1467,30 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleveland clinic data import preliminary version
</commit_message>
<xml_diff>
--- a/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
+++ b/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
@@ -473,10 +473,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -863,9 +863,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -877,7 +877,7 @@
     <col min="5" max="5" width="9.5" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" customWidth="1"/>
     <col min="9" max="9" width="39.5" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
     <col min="12" max="12" width="8.83203125" customWidth="1"/>
@@ -919,19 +919,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
@@ -1151,19 +1151,19 @@
       </c>
     </row>
     <row r="22" spans="1:12" s="2" customFormat="1">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="5" t="s">
@@ -1292,22 +1292,22 @@
       <c r="J32">
         <v>20</v>
       </c>
-      <c r="L32" s="7"/>
+      <c r="L32" s="6"/>
     </row>
     <row r="34" spans="1:16" s="2" customFormat="1">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="5" t="s">
@@ -1376,11 +1376,11 @@
       <c r="J40">
         <v>10</v>
       </c>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
     </row>
     <row r="41" spans="1:16">
       <c r="H41" t="s">
@@ -1392,7 +1392,7 @@
       <c r="J41">
         <v>20</v>
       </c>
-      <c r="L41" s="7"/>
+      <c r="L41" s="6"/>
     </row>
     <row r="42" spans="1:16">
       <c r="H42" t="s">
@@ -1404,7 +1404,7 @@
       <c r="J42">
         <v>30</v>
       </c>
-      <c r="L42" s="7"/>
+      <c r="L42" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
cleveland clinic question/answer identifiers are imported
</commit_message>
<xml_diff>
--- a/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
+++ b/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="109">
   <si>
     <t>id</t>
   </si>
@@ -340,10 +340,13 @@
     <t>qx_exercise_longjump</t>
   </si>
   <si>
-    <t>answer_exercise_longjump</t>
-  </si>
-  <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>answer_exercise_longjump_feet</t>
+  </si>
+  <si>
+    <t>answer_exercise_longjump_inches</t>
   </si>
 </sst>
 </file>
@@ -865,7 +868,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1167,7 +1170,7 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
         <v>77</v>
@@ -1276,7 +1279,7 @@
         <v>31</v>
       </c>
       <c r="I31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J31">
         <v>10</v>
@@ -1287,7 +1290,7 @@
         <v>32</v>
       </c>
       <c r="I32" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J32">
         <v>20</v>

</xml_diff>

<commit_message>
cleveland clinic conditions is imported
</commit_message>
<xml_diff>
--- a/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
+++ b/api/test/fixtures/import-export/ccf/ccf-questions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="120">
   <si>
     <t>id</t>
   </si>
@@ -280,9 +280,6 @@
     <t>qx_tv_size_key</t>
   </si>
   <si>
-    <t>What is size of your largest TV?</t>
-  </si>
-  <si>
     <t>32 or less</t>
   </si>
   <si>
@@ -347,6 +344,42 @@
   </si>
   <si>
     <t>answer_exercise_longjump_inches</t>
+  </si>
+  <si>
+    <t>What is the size of your primary TV?</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>qx_2nd_tv_size_key</t>
+  </si>
+  <si>
+    <t>What is the size of your secondary TV?</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>answer_2nd_tv_size_32_less</t>
+  </si>
+  <si>
+    <t>answer_2nd_tv_size_33_66</t>
+  </si>
+  <si>
+    <t>answer_2nd_tv_size_66_more</t>
+  </si>
+  <si>
+    <t>qx_has_second_tv_key</t>
+  </si>
+  <si>
+    <t>Do you have a secondary TV?</t>
+  </si>
+  <si>
+    <t>answer_has_second_tv_key_yes</t>
+  </si>
+  <si>
+    <t>answer_has_second_tv_key_no</t>
   </si>
 </sst>
 </file>
@@ -416,8 +449,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -481,7 +530,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -506,6 +555,14 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -530,6 +587,14 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -864,11 +929,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1170,7 +1235,7 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
         <v>77</v>
@@ -1244,10 +1309,10 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" t="s">
         <v>25</v>
@@ -1256,7 +1321,7 @@
         <v>30</v>
       </c>
       <c r="I29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J29">
         <v>10</v>
@@ -1267,10 +1332,10 @@
         <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F31" t="s">
         <v>26</v>
@@ -1279,7 +1344,7 @@
         <v>31</v>
       </c>
       <c r="I31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J31">
         <v>10</v>
@@ -1290,7 +1355,7 @@
         <v>32</v>
       </c>
       <c r="I32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J32">
         <v>20</v>
@@ -1320,16 +1385,16 @@
         <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="F36" t="s">
         <v>17</v>
       </c>
       <c r="H36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J36">
         <v>10</v>
@@ -1337,10 +1402,10 @@
     </row>
     <row r="37" spans="1:16">
       <c r="H37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J37" s="1">
         <v>20</v>
@@ -1348,10 +1413,10 @@
     </row>
     <row r="38" spans="1:16">
       <c r="H38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J38" s="1">
         <v>30</v>
@@ -1362,19 +1427,19 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" t="s">
         <v>93</v>
-      </c>
-      <c r="C40" t="s">
-        <v>94</v>
       </c>
       <c r="F40" t="s">
         <v>10</v>
       </c>
       <c r="H40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J40">
         <v>10</v>
@@ -1387,10 +1452,10 @@
     </row>
     <row r="41" spans="1:16">
       <c r="H41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J41">
         <v>20</v>
@@ -1399,15 +1464,101 @@
     </row>
     <row r="42" spans="1:16">
       <c r="H42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J42">
         <v>30</v>
       </c>
       <c r="L42" s="6"/>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" t="s">
+        <v>117</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" t="s">
+        <v>119</v>
+      </c>
+      <c r="H44" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" t="s">
+        <v>118</v>
+      </c>
+      <c r="J44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="4"/>
+      <c r="H45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" t="s">
+        <v>119</v>
+      </c>
+      <c r="J45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" t="s">
+        <v>86</v>
+      </c>
+      <c r="I47" t="s">
+        <v>113</v>
+      </c>
+      <c r="J47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="H48" t="s">
+        <v>87</v>
+      </c>
+      <c r="I48" t="s">
+        <v>114</v>
+      </c>
+      <c r="J48" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="8:10">
+      <c r="H49" t="s">
+        <v>88</v>
+      </c>
+      <c r="I49" t="s">
+        <v>115</v>
+      </c>
+      <c r="J49" s="1">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>